<commit_message>
Insert data into stores table
</commit_message>
<xml_diff>
--- a/store-data.xlsx
+++ b/store-data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Web-Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26685A41-14D0-46D7-964D-DE9BC7276BA0}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A321648B-C484-43B6-9834-B00DA0E8EAA3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7485" xr2:uid="{4A5A47EB-D695-48FD-8865-D15FF23C3366}"/>
   </bookViews>
@@ -678,19 +678,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE50CC4-EE0D-4642-A8ED-60EB00CBAD66}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2:N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="61.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" customWidth="1"/>
+    <col min="3" max="3" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -701,7 +702,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -711,8 +712,12 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N2" t="str">
+        <f>"INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"');"</f>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Morico - Contemporary Japanese Lifestyle - Lê Lợi ',' 30 Lê Lợi, P. Bến Nghé, Quận 1 , TP. HCM ','https://images.foody.vn/res/g1/595/prof/s640x400/foody-upload-api-foody-mobile-10-jpg-180508140146.jpg');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -722,8 +727,12 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N3" t="str">
+        <f t="shared" ref="N3:N37" si="0">"INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('"&amp;A3&amp;"','"&amp;B3&amp;"','"&amp;C3&amp;"');"</f>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Monkey In Black Cafe ',' 2 chi nhánh ','https://images.foody.vn/res/g9/89822/prof/s640x400/foody-mobile-zas-jpg-258-636086627918162406.jpg');</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -733,8 +742,12 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Oromia Coffee - Nam Kỳ Khởi Nghĩa ',' 193A/D3 Nam Kỳ Khởi Nghĩa, Quận 3 , TP. HCM ','https://images.foody.vn/res/g12/112158/prof/s640x400/foody-mobile-1-jpg-194-636289977329979410.jpg');</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -744,8 +757,12 @@
       <c r="C5" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Starbucks Coffee - HCM ',' 25 chi nhánh ','https://images.foody.vn/res/g2/15031/prof/s640x400/foody-mobile-mobile-jpg-409-635744522405981690.jpg');</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -755,8 +772,12 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Morico - Modern Japanese - Food, Sushi &amp; Dessert ',' 3 chi nhánh ','https://images.foody.vn/res/g1/742/prof/s640x400/foody-upload-api-foody-mobile-9-jpg-180508140028.jpg');</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -766,8 +787,12 @@
       <c r="C7" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Partea ',' 2 chi nhánh ','https://images.foody.vn/res/g8/77729/prof/s640x400/foody-mobile-12-jpg-868-636171531644694064.jpg');</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -777,8 +802,12 @@
       <c r="C8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Đen Đá Cafe ',' 7 chi nhánh ','https://images.foody.vn/res/g12/110335/prof/s640x400/foody-mobile-mhfo7qz6-jpg-187-636130047827225698.jpg');</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
@@ -788,8 +817,12 @@
       <c r="C9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Morico - Contemporary Japanese Lifestyle ',' 2 chi nhánh ','https://images.foody.vn/res/g1/900/prof/s640x400/foody-upload-api-foody-mobile-7-jpg-180508135106.jpg');</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -799,8 +832,12 @@
       <c r="C10" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Paris Baguette - Cao Thắng ',' 1 Cao Thắng, P. 2, Quận 3 , TP. HCM ','https://images.foody.vn/res/g1/4336/prof/s640x400/foody-upload-api-foody-mobile--b5e49debee037df4559-180704101653.jpg');</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
@@ -810,8 +847,12 @@
       <c r="C11" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Phúc Long Coffee &amp; Tea Express ',' 30 chi nhánh ','https://images.foody.vn/res/g9/87015/prof/s640x400/foody-mobile-phuc-long-ly-tu-tron-343-635791628128985595.jpg');</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -821,8 +862,12 @@
       <c r="C12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Trà Sữa Gong Cha - 貢茶 - Hồ Tùng Mậu ',' 83 Hồ Tùng Mậu, Quận 1 , TP. HCM ','https://images.foody.vn/res/g10/96530/prof/s640x400/foody-mobile-gong-cha2-jpg-305-636173909122516269.jpg');</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -832,8 +877,12 @@
       <c r="C13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Moon Fast Food - Món Hàn - Xuân Hồng ',' 53 Xuân Hồng, P. 12, Quận Tân Bình , TP. HCM ','https://images.foody.vn/res/g8/71782/prof/s640x400/foody-mobile-mon-fastfood-mb-jpg-441-635895077676626146.jpg');</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>37</v>
       </c>
@@ -843,8 +892,12 @@
       <c r="C14" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Morico - Contemporary Japanese Lifestyle - Vincom Center ',' Tầng B3 Vincom Center, 70 - 72 Lê Thánh Tôn, P. Bến Nghé, Quận 1 , TP. HCM ','https://images.foody.vn/res/g1/742/prof/s640x400/foody-upload-api-foody-mobile-9-jpg-180508140028.jpg');</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -854,8 +907,12 @@
       <c r="C15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Paris Baguette ',' 4 chi nhánh ','https://images.foody.vn/res/g1/4336/prof/s640x400/foody-upload-api-foody-mobile--b5e49debee037df4559-180704101653.jpg');</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>34</v>
       </c>
@@ -865,8 +922,12 @@
       <c r="C16" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Moon Fast Food - Món Hàn - Xuân Hồng ',' 53 Xuân Hồng, P. 12, Quận Tân Bình , TP. HCM ','https://images.foody.vn/res/g8/71782/prof/s640x400/foody-mobile-mon-fastfood-mb-jpg-441-635895077676626146.jpg');</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -876,8 +937,12 @@
       <c r="C17" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Fly Cupcake ',' 2 chi nhánh ','https://images.foody.vn/res/g1/6676/prof/s640x400/foody-mobile-flycupcake-jpg-612-635657179559706401.jpg');</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>43</v>
       </c>
@@ -887,8 +952,12 @@
       <c r="C18" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Star Kitchen ',' 3 chi nhánh ','https://images.foody.vn/res/g10/90625/prof/s640x400/foody-upload-api-foody-mobile-21-jpg-181114113351.jpg');</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>45</v>
       </c>
@@ -898,8 +967,12 @@
       <c r="C19" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Dallas Cakes &amp; Coffee ',' 5 chi nhánh ','https://images.foody.vn/res/g1/9138/prof/s640x400/foody-upload-api-foody-mobile-3-jpg-180409101750.jpg');</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>48</v>
       </c>
@@ -909,8 +982,12 @@
       <c r="C20" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Buffet Windsor - Cafe Central An Dong - Windsor Plaza ',' Windsor Plaza, 18 An Dương Vương, Quận 5 , TP. HCM ','https://images.foody.vn/res/g1/8/prof/s640x400/foody-mobile-dpxxrdae-jpg-176-635851879399811855.jpg');</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>51</v>
       </c>
@@ -920,8 +997,12 @@
       <c r="C21" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống TOUS les JOURS SG ',' 6 chi nhánh ','https://images.foody.vn/res/g1/520/prof/s640x400/foody-upload-api-foody-mobile-tlj-jpg-180521103523.jpg');</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>54</v>
       </c>
@@ -931,8 +1012,12 @@
       <c r="C22" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Chewy Chewy - Cafe &amp; Bánh - Trần Hưng Đạo ',' 34 Trần Hưng Đạo, P. Phạm Ngũ Lão, Quận 1 , TP. HCM ','https://images.foody.vn/res/g1/4139/prof/s640x400/foody-upload-api-foody-mobile-18-jpg-181023082644.jpg');</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>57</v>
       </c>
@@ -942,8 +1027,12 @@
       <c r="C23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Bánh Bao Thọ Phát - Nguyễn Tri Phương ',' 78 Nguyễn Tri Phương, P. 7, Quận 5 , TP. HCM ','https://images.foody.vn/res/g1/3100/prof/s640x400/foody-mobile-tho-phat-jpg-980-636044605184486406.jpg');</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>60</v>
       </c>
@@ -953,8 +1042,12 @@
       <c r="C24" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Cheesecake Ngon ',' 2 chi nhánh ','https://images.foody.vn/res/g5/44454/prof/s640x400/foody-mobile-cheese-cake-jpg-576-636119657716824761.jpg');</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>62</v>
       </c>
@@ -964,8 +1057,12 @@
       <c r="C25" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('TacoLeo - Ẩm Thực Mexico - Cao Bá Nhạ ',' 20 Cao Bá Nhạ, P. Nguyễn Cư Trinh, Quận 1 , TP. HCM ','https://images.foody.vn/res/g5/49674/prof/s640x400/foody-mobile-cao-ba-nha-jpg.jpg');</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>65</v>
       </c>
@@ -975,8 +1072,12 @@
       <c r="C26" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Sumo BBQ - Buffet Lẩu &amp; Nướng ',' 11 chi nhánh ','https://images.foody.vn/res/g1/4074/prof/s640x400/foody-mobile-12-jpg-340-636169623888144042.jpg');</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>68</v>
       </c>
@@ -986,8 +1087,12 @@
       <c r="C27" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Red Chilli Seafood Buffet - CHLOE Gallery ',' 2 - 6 Phan Văn Chương, Phú Mỹ Hưng, Quận 7 , TP. HCM ','https://images.foody.vn/res/g1/562/prof/s640x400/foody-mobile-109-jpg-361-635858632711885387.jpg');</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>71</v>
       </c>
@@ -997,8 +1102,12 @@
       <c r="C28" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Sushi Dining AOI - Món Nhật ',' 53 - 55 Bà Huyện Thanh Quan, P. 6, Quận 3 , TP. HCM ','https://images.foody.vn/res/g1/726/prof/s640x400/foody-mobile-sushi-set-aoi-jpg-270-636317608417017315.jpg');</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
@@ -1008,8 +1117,12 @@
       <c r="C29" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Hana Buffet ',' 6 chi nhánh ','https://images.foody.vn/res/g2/13986/prof/s640x400/foody-mobile-hana-buffet-pvc-mb-j-201-635924466203859693.jpg');</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
@@ -1019,8 +1132,12 @@
       <c r="C30" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Buffet Windsor - Cafe Central An Dong - Windsor Plaza ',' Windsor Plaza, 18 An Dương Vương, Quận 5 , TP. HCM ','https://images.foody.vn/res/g1/8/prof/s640x400/foody-mobile-dpxxrdae-jpg-176-635851879399811855.jpg');</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>76</v>
       </c>
@@ -1030,8 +1147,12 @@
       <c r="C31" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('L'angfarm Buffet - Trần Hưng Đạo ',' 771 - 773 - 775 Trần Hưng Đạo, P. 1, Quận 5 , TP. HCM ','https://images.foody.vn/res/g22/215893/prof/s640x400/2018123152530-langfarm-buffet-tran-hung-dao-copy.jpg');</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>79</v>
       </c>
@@ -1041,8 +1162,12 @@
       <c r="C32" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('La Brasserie Restaurant - Hotel Nikko Saigon ',' Hotel Nikko Saigon, 235 Nguyễn Văn Cừ, Quận 1, Quận 1 , TP. HCM ','https://images.foody.vn/res/g4/33141/prof/s640x400/2017619161034-img_2388.jpg');</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>82</v>
       </c>
@@ -1052,8 +1177,12 @@
       <c r="C33" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống Hoàng Yến Buffet ',' 5 chi nhánh ','https://images.foody.vn/res/g1/305/prof/s640x400/foody-mobile-dsc_0886-jpg-219-636118800111396860.jpg');</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>84</v>
       </c>
@@ -1063,8 +1192,12 @@
       <c r="C34" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Cheap Eats - Seafood BBQ Buffet ',' Tầng 5, 9 Nguyễn Trãi, P. Bến Thành, Quận 1 , TP. HCM ','https://images.foody.vn/res/g26/255427/prof/s640x400/foody-mobile-1-jpg-112-636258618783661123.jpg');</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>87</v>
       </c>
@@ -1074,8 +1207,12 @@
       <c r="C35" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Hệ thống King BBQ ',' 24 chi nhánh ','https://images.foody.vn/res/g5/46902/prof/s640x400/foody-mobile-gff-jpg-282-635768935243754658.jpg');</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>90</v>
       </c>
@@ -1085,8 +1222,12 @@
       <c r="C36" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="N36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Parkview Buffet - New World Saigon Hotel ',' New World Saigon Hotel, 76 Lê Lai, P. Bến Nghé, Quận 1 , TP. HCM ','https://images.foody.vn/res/g2/15012/prof/s640x400/2017539570-_parkview-2-.jpg');</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>93</v>
       </c>
@@ -1095,6 +1236,10 @@
       </c>
       <c r="C37" t="s">
         <v>95</v>
+      </c>
+      <c r="N37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO `stores` (`name`, `address`, `image`) VALUES ('Fujiya Restaurant - Yakiniku Nabe Buffet ',' B3-01 Vincom Center, 72 Lê Thánh Tôn, Quận 1 , TP. HCM ','https://images.foody.vn/res/g10/94289/prof/s640x400/foody-upload-api-foody-mobile-2-jpg-180602081629.jpg');</v>
       </c>
     </row>
   </sheetData>

</xml_diff>